<commit_message>
redid 'type the senetence and get a correct mark' logic, as it seemed to have broken
</commit_message>
<xml_diff>
--- a/content/common_1000/common_1000.xlsx
+++ b/content/common_1000/common_1000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\Learn_Czech\content\common_1000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7DD4AF-A54A-4AF7-9993-93191FACC7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D3237C-3517-4D9E-ADB9-BB884BAE887A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16230" yWindow="1245" windowWidth="33270" windowHeight="19470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16962,8 +16962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A941" workbookViewId="0">
-      <selection activeCell="I946" sqref="I946"/>
+    <sheetView tabSelected="1" topLeftCell="A987" workbookViewId="0">
+      <selection activeCell="H994" sqref="H994"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17342,7 +17342,7 @@
         <v>4369</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -17631,7 +17631,7 @@
         <v>4383</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>109</v>
       </c>
@@ -19894,7 +19894,7 @@
         <v>3071</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>483</v>
       </c>
@@ -19954,7 +19954,7 @@
         <v>3077</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>492</v>
       </c>
@@ -20694,7 +20694,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>595</v>
       </c>
@@ -21414,7 +21414,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>699</v>
       </c>
@@ -22094,7 +22094,7 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>797</v>
       </c>
@@ -23314,7 +23314,7 @@
         <v>3417</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>972</v>
       </c>
@@ -24134,7 +24134,7 @@
         <v>3498</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>1088</v>
       </c>
@@ -24314,7 +24314,7 @@
         <v>3516</v>
       </c>
     </row>
-    <row r="392" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>1114</v>
       </c>
@@ -24574,7 +24574,7 @@
         <v>3543</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>1149</v>
       </c>
@@ -25108,7 +25108,7 @@
         <v>3591</v>
       </c>
     </row>
-    <row r="432" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>1227</v>
       </c>
@@ -25188,7 +25188,7 @@
         <v>3599</v>
       </c>
     </row>
-    <row r="436" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>1239</v>
       </c>
@@ -26828,7 +26828,7 @@
         <v>3763</v>
       </c>
     </row>
-    <row r="518" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>909</v>
       </c>
@@ -27008,7 +27008,7 @@
         <v>3782</v>
       </c>
     </row>
-    <row r="527" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>1502</v>
       </c>
@@ -27404,7 +27404,7 @@
         <v>3823</v>
       </c>
     </row>
-    <row r="547" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>1560</v>
       </c>
@@ -27424,7 +27424,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="548" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>1563</v>
       </c>
@@ -28104,7 +28104,7 @@
         <v>3893</v>
       </c>
     </row>
-    <row r="582" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>1662</v>
       </c>
@@ -28424,7 +28424,7 @@
         <v>3925</v>
       </c>
     </row>
-    <row r="598" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>1708</v>
       </c>
@@ -28604,7 +28604,7 @@
         <v>3943</v>
       </c>
     </row>
-    <row r="607" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>1734</v>
       </c>
@@ -28624,7 +28624,7 @@
         <v>3945</v>
       </c>
     </row>
-    <row r="608" spans="1:6" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>1737</v>
       </c>
@@ -28814,7 +28814,7 @@
         <v>4061</v>
       </c>
     </row>
-    <row r="619" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
         <v>1769</v>
       </c>
@@ -29358,7 +29358,7 @@
         <v>4952</v>
       </c>
     </row>
-    <row r="651" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="651" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
         <v>1861</v>
       </c>
@@ -29460,7 +29460,7 @@
         <v>4958</v>
       </c>
     </row>
-    <row r="657" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="657" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
         <v>1879</v>
       </c>
@@ -29630,7 +29630,7 @@
         <v>4968</v>
       </c>
     </row>
-    <row r="667" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="667" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
         <v>1909</v>
       </c>
@@ -29953,7 +29953,7 @@
         <v>4985</v>
       </c>
     </row>
-    <row r="686" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="686" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A686" t="s">
         <v>1964</v>
       </c>
@@ -30327,7 +30327,7 @@
         <v>5005</v>
       </c>
     </row>
-    <row r="708" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
         <v>2026</v>
       </c>
@@ -30990,7 +30990,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="747" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="747" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A747" t="s">
         <v>2138</v>
       </c>
@@ -31211,7 +31211,7 @@
         <v>5055</v>
       </c>
     </row>
-    <row r="760" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="760" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A760" t="s">
         <v>2176</v>
       </c>
@@ -31789,7 +31789,7 @@
         <v>5088</v>
       </c>
     </row>
-    <row r="794" spans="1:5" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="794" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
         <v>2276</v>
       </c>
@@ -32027,7 +32027,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="808" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="808" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
         <v>2318</v>
       </c>
@@ -32469,7 +32469,7 @@
         <v>5126</v>
       </c>
     </row>
-    <row r="834" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="834" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A834" t="s">
         <v>777</v>
       </c>
@@ -32503,7 +32503,7 @@
         <v>5128</v>
       </c>
     </row>
-    <row r="836" spans="1:5" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="836" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A836" t="s">
         <v>2400</v>
       </c>
@@ -32894,7 +32894,7 @@
         <v>5150</v>
       </c>
     </row>
-    <row r="859" spans="1:5" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="859" spans="1:5" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
         <v>2465</v>
       </c>
@@ -32996,7 +32996,7 @@
         <v>5156</v>
       </c>
     </row>
-    <row r="865" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="865" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A865" t="s">
         <v>2483</v>
       </c>
@@ -33285,7 +33285,7 @@
         <v>5173</v>
       </c>
     </row>
-    <row r="882" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="882" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
         <v>2531</v>
       </c>
@@ -33421,7 +33421,7 @@
         <v>5181</v>
       </c>
     </row>
-    <row r="890" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="890" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A890" t="s">
         <v>2555</v>
       </c>
@@ -33523,7 +33523,7 @@
         <v>5187</v>
       </c>
     </row>
-    <row r="896" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="896" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
         <v>2571</v>
       </c>
@@ -33659,7 +33659,7 @@
         <v>5195</v>
       </c>
     </row>
-    <row r="904" spans="1:5" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="904" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
         <v>2594</v>
       </c>
@@ -33795,7 +33795,7 @@
         <v>5203</v>
       </c>
     </row>
-    <row r="912" spans="1:5" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="912" spans="1:5" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A912" t="s">
         <v>2617</v>
       </c>
@@ -33931,7 +33931,7 @@
         <v>5211</v>
       </c>
     </row>
-    <row r="920" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="920" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
         <v>2640</v>
       </c>
@@ -34169,7 +34169,7 @@
         <v>5225</v>
       </c>
     </row>
-    <row r="934" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="934" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A934" t="s">
         <v>2680</v>
       </c>
@@ -34305,7 +34305,7 @@
         <v>5233</v>
       </c>
     </row>
-    <row r="942" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="942" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
         <v>2703</v>
       </c>

</xml_diff>